<commit_message>
Upgrade create-issues script to accept arguments
This improves usability of the script and avoids having to edit
parts of it for each new release. It also adds a --dry-run
option to test the script without creating the issues
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS_11_2020.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS_11_2020.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10808"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlc47243\Documents\mantid-development\mantid-docs\documents\Project-Management\Tools\RoadmapUpdate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmn58364/Code/git/mantidproject/documents/Project-Management/Tools/RoadmapUpdate/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BCD475-22E0-4C47-A9C4-3F2B18E78542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1033" yWindow="467" windowWidth="27767" windowHeight="17533"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -26,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -71,18 +73,6 @@
     <t>small</t>
   </si>
   <si>
-    <t>Make sure that inputs and outputs work sensibly, stress test with some bad inputs (e.g. letters in a numeric input)
-See http://docs.mantidproject.org/v3.7.2/interfaces/SampleTransmissionCalculator.html</t>
-  </si>
-  <si>
-    <t>Make sure that inputs and outputs work sensibly, stress test with some bad inputs (e.g. letters in a numeric input)
-See http://docs.mantidproject.org/v3.12.0/interfaces/TOF%20Converter.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Follow the directions at: http://developer.mantidproject.org/Testing/IndirectInelastic/IndirectInelasticAcceptanceTests.html
-</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -105,13 +95,6 @@
   </si>
   <si>
     <t>For testing procedures see http://developer.mantidproject.org/Testing/ReflectometryGUI/ReflectometryGUITests.html</t>
-  </si>
-  <si>
-    <t>http://developer.mantidproject.org/Testing/Core/Core.html</t>
-  </si>
-  <si>
-    <t>See instructions at https://developer.mantidproject.org/Testing/MuonAnalysis_test_guides/index.html
-http://developer.mantidproject.org/Testing/MuonInterface/MuonTesting.html</t>
   </si>
   <si>
     <t>* Follow the examples at http://docs.mantidproject.org/nightly/concepts/WorkspaceGroup.html 
@@ -225,11 +208,30 @@
 * Open up the basic course (docs/html/tutorials/mantid_basic_course/index.html)
 * Check that the pages in there make sense</t>
   </si>
+  <si>
+    <t>Make sure that inputs and outputs work sensibly, stress test with some bad inputs (e.g. letters in a numeric input)
+See https://docs.mantidproject.org/interfaces/TOF%20Converter.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follow the directions at: https://developer.mantidproject.org/Testing/IndirectInelastic/IndirectInelasticAcceptanceTests.html
+</t>
+  </si>
+  <si>
+    <t>https://developer.mantidproject.org/Testing/Core/Core.html</t>
+  </si>
+  <si>
+    <t>See instructions at https://developer.mantidproject.org/Testing/MuonAnalysis_test_guides/index.html
+https://developer.mantidproject.org/Testing/MuonInterface/MuonTesting.html</t>
+  </si>
+  <si>
+    <t>Make sure that inputs and outputs work sensibly, stress test with some bad inputs (e.g. letters in a numeric input)
+See https://docs.mantidproject.org/interfaces/SampleTransmissionCalculator.html</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -896,6 +898,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -931,6 +950,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1106,22 +1142,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46" style="1" customWidth="1"/>
-    <col min="2" max="2" width="72.703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.87890625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.1171875" style="1"/>
+    <col min="2" max="2" width="72.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1129,306 +1165,306 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="172" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.350000000000001" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="100.35" x14ac:dyDescent="0.5">
-      <c r="A17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="C18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="229.35" x14ac:dyDescent="0.5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="240" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://developer.mantidproject.org/Testing/IndirectInelastic/IndirectInelasticAcceptanceTests.html_x000a_"/>
-    <hyperlink ref="B7" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://developer.mantidproject.org/Testing/IndirectInelastic/IndirectInelasticAcceptanceTests.html" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>[issue_templateupdate.xlsx]assignees!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>C22:C27</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>assignees!$A$2:$A$5</xm:f>
           </x14:formula1>
@@ -1441,70 +1477,70 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <f>COUNTIF(issues!$C:$C,assignees!A2)</f>
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <f>COUNTIF(issues!$C:$C,assignees!A3)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <f>COUNTIF(issues!$C:$C,assignees!A4)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <f>COUNTIF(issues!$C:$C,assignees!A5)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
     </row>
-    <row r="15" spans="1:2" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="A4:C16">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:C16">
     <sortCondition descending="1" ref="B4:B27"/>
   </sortState>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
Add empty Assignee column to spreadsheet to pass create_issue script
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS_11_2020.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template_ISIS_11_2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmn58364/Code/git/mantidproject/documents/Project-Management/Tools/RoadmapUpdate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmurphy/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BCD475-22E0-4C47-A9C4-3F2B18E78542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B30162-0E70-FB49-8A8F-DB805BEEA36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="500" windowWidth="32420" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
   <si>
     <t>Title</t>
   </si>
@@ -226,6 +226,9 @@
   <si>
     <t>Make sure that inputs and outputs work sensibly, stress test with some bad inputs (e.g. letters in a numeric input)
 See https://docs.mantidproject.org/interfaces/SampleTransmissionCalculator.html</t>
+  </si>
+  <si>
+    <t>Assignee</t>
   </si>
 </sst>
 </file>
@@ -1146,7 +1149,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1166,6 +1169,9 @@
       </c>
       <c r="C1" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>

</xml_diff>